<commit_message>
Test detection matos + MAJ doc excel
</commit_message>
<xml_diff>
--- a/todo_vUltime.xlsx
+++ b/todo_vUltime.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="137">
   <si>
     <t xml:space="preserve">-&gt; explosion de bulo - attaque en l'air - transformation </t>
   </si>
@@ -364,13 +364,76 @@
   </si>
   <si>
     <t xml:space="preserve">gameplay =&gt; quete </t>
+  </si>
+  <si>
+    <t>Fait, on peut ajouter autant de logos qu'on veut. A éttendre pour pouvoir gérer la zappabilité, le son, pk pas la video</t>
+  </si>
+  <si>
+    <t>Vraiment trop dur… Tenté par Jagueu</t>
+  </si>
+  <si>
+    <t>Très dur</t>
+  </si>
+  <si>
+    <t>Commentaire</t>
+  </si>
+  <si>
+    <t>Guillaume va tester l'API cpu-z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peut etre trop amusant. </t>
+  </si>
+  <si>
+    <t>A voir si fonctions de flou possibles via XNA</t>
+  </si>
+  <si>
+    <t>Refonte graphique: la barre existe deja</t>
+  </si>
+  <si>
+    <t>Subition</t>
+  </si>
+  <si>
+    <t>A faire dés que j'ai la motivation (guillaume)</t>
+  </si>
+  <si>
+    <t>En créant un dossier dans My Games/My Erasme/ My Bulo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fait, Valeur par defaut + réglable dans le XML + zappable avec TAB </t>
+  </si>
+  <si>
+    <t>fait, a déclarer  dans le XML, autant d'étapes que l'on veut, vitesse reglable, s'arette lorsque le texte a fini de s'afficher. (faudrais passer cette derniére option en réglable dans le XML, pour certaines situations spéciales (eramse a peur, par exemple) où l'anim doit continuer)</t>
+  </si>
+  <si>
+    <t>DUUUUUR</t>
+  </si>
+  <si>
+    <t>Déjà tenté, déjà échoué</t>
+  </si>
+  <si>
+    <t>dur</t>
+  </si>
+  <si>
+    <t>Over dur</t>
+  </si>
+  <si>
+    <t>Pas trop dur a coder, mais dur a rendre beau</t>
+  </si>
+  <si>
+    <t>pas trop dur?</t>
+  </si>
+  <si>
+    <t>Facile</t>
+  </si>
+  <si>
+    <t>DUR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -378,13 +441,45 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -399,8 +494,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -416,7 +529,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -704,550 +817,646 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F143"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="59.25" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="57.7109375" customWidth="1"/>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="172.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="57.7109375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="3"/>
+    <col min="3" max="3" width="10" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="55.140625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="63.28515625" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" s="2" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="E1" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="4" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="4">
         <v>100</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="4" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="E2" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="6" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="6">
         <v>9000</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="6" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="E3" s="6" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="D4" t="s">
+      <c r="C4" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="E4" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="D5" t="s">
+      <c r="C5" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="E5" s="3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="3" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:5" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="3" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="E7" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="3" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="9" spans="1:5" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="D9" t="s">
+      <c r="C9" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="E9" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="D10" t="s">
+      <c r="C10" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="E10" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="D11" t="s">
+      <c r="C11" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="E11" s="3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="C12" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="D13" t="s">
+      <c r="C13" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="E13" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="D14" t="s">
+      <c r="C14" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="15" spans="1:5" s="1" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="E15" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" s="5" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="E16" s="5" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" s="6" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="C17" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="D18" t="s">
+      <c r="C18" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="D18" s="3" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="19" spans="1:5" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="D19" t="s">
+      <c r="C19" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="D19" s="3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="20" spans="1:5" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="D20" t="s">
+      <c r="C20" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="D20" s="3" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="21" spans="1:5" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="D21" t="s">
+      <c r="C21" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="D21" s="3" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="22" spans="1:5" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="D22" t="s">
+      <c r="C22" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="D22" s="3" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="23" spans="1:5" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="C23" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="25" spans="1:5" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="D25" t="s">
+      <c r="C25" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="D25" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="26" spans="1:5" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="D26" t="s">
+      <c r="C26" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="D26" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="27" spans="1:5" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="3" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="28" spans="1:5" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="29" spans="1:5" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="30" spans="1:5" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="3" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="31" spans="1:5" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+    <row r="47" spans="1:1" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+    <row r="48" spans="1:1" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D49" t="s">
+    <row r="49" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D49" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B50" t="s">
+    <row r="50" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+    <row r="51" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+    <row r="53" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+    <row r="54" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+    <row r="55" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+    <row r="56" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B57" t="s">
+    <row r="57" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B57" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B58" t="s">
+    <row r="58" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B58" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B59" t="s">
+    <row r="59" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B59" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B60" t="s">
+    <row r="60" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B60" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+    <row r="61" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
+    <row r="62" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
+    <row r="63" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
+    <row r="64" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
+    <row r="65" spans="1:1" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
+    <row r="66" spans="1:1" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
+    <row r="67" spans="1:1" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
+    <row r="68" spans="1:1" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
+    <row r="69" spans="1:1" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
+    <row r="71" spans="1:1" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
+    <row r="73" spans="1:1" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
+    <row r="75" spans="1:1" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
+    <row r="77" spans="1:1" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
+    <row r="79" spans="1:1" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
+    <row r="81" spans="1:1" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
+    <row r="84" spans="1:1" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
+    <row r="85" spans="1:1" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
+    <row r="87" spans="1:1" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
+    <row r="88" spans="1:1" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
+    <row r="89" spans="1:1" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
+    <row r="90" spans="1:1" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
+    <row r="91" spans="1:1" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
+    <row r="92" spans="1:1" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
+    <row r="93" spans="1:1" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
+    <row r="94" spans="1:1" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
+    <row r="95" spans="1:1" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
+    <row r="96" spans="1:1" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
+    <row r="97" spans="1:1" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
+    <row r="98" spans="1:1" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
+    <row r="99" spans="1:1" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
+    <row r="100" spans="1:1" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
+    <row r="101" spans="1:1" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
+    <row r="102" spans="1:1" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
+    <row r="103" spans="1:1" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
+    <row r="104" spans="1:1" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
+    <row r="105" spans="1:1" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
+    <row r="106" spans="1:1" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
+    <row r="108" spans="1:1" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
+    <row r="109" spans="1:1" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
+    <row r="111" spans="1:1" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
+    <row r="112" spans="1:1" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
+    <row r="115" spans="1:1" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A115" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
+    <row r="118" spans="1:1" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A118" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="143" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F143" t="s">
+    <row r="143" spans="6:6" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F143" s="3" t="s">
         <v>58</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1257,7 +1466,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1269,7 +1478,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Maj du todo_vUltime.xlsx Ajout d'un fichier de test Effects/TestEffect.fx
</commit_message>
<xml_diff>
--- a/todo_vUltime.xlsx
+++ b/todo_vUltime.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="138">
   <si>
     <t xml:space="preserve">-&gt; explosion de bulo - attaque en l'air - transformation </t>
   </si>
@@ -369,24 +369,15 @@
     <t>Fait, on peut ajouter autant de logos qu'on veut. A éttendre pour pouvoir gérer la zappabilité, le son, pk pas la video</t>
   </si>
   <si>
-    <t>Vraiment trop dur… Tenté par Jagueu</t>
-  </si>
-  <si>
     <t>Très dur</t>
   </si>
   <si>
     <t>Commentaire</t>
   </si>
   <si>
-    <t>Guillaume va tester l'API cpu-z</t>
-  </si>
-  <si>
     <t xml:space="preserve">Peut etre trop amusant. </t>
   </si>
   <si>
-    <t>A voir si fonctions de flou possibles via XNA</t>
-  </si>
-  <si>
     <t>Refonte graphique: la barre existe deja</t>
   </si>
   <si>
@@ -408,9 +399,6 @@
     <t>DUUUUUR</t>
   </si>
   <si>
-    <t>Déjà tenté, déjà échoué</t>
-  </si>
-  <si>
     <t>dur</t>
   </si>
   <si>
@@ -427,6 +415,21 @@
   </si>
   <si>
     <t>DUR</t>
+  </si>
+  <si>
+    <t>Guillaume va tester l'API cpu-z ==&gt; API CPU-Z payante. Test avec WMI, presque bien. Pour l'instant affiche le modèle aproximatif dans la console.</t>
+  </si>
+  <si>
+    <t>A voir si fonctions de flou possibles via XNA ==&gt; Utiliser des fichiers effects, avec du code et des shaders ultra durs dedans (.fx)</t>
+  </si>
+  <si>
+    <t>Ultra dur</t>
+  </si>
+  <si>
+    <t>Vraiment trop dur… Tenté par Jagueu ==&gt; Finalement Jagueu a réussi. Maintenant faut y mettre des trucs amusants</t>
+  </si>
+  <si>
+    <t>Déjà tenté, déjà échoué. A retenter</t>
   </si>
 </sst>
 </file>
@@ -817,8 +820,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="59.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -845,7 +848,7 @@
         <v>73</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="4" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -865,32 +868,32 @@
         <v>116</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="6" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+    <row r="3" spans="1:5" s="4" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="4">
         <v>9000</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="4" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>120</v>
+      <c r="E4" s="4" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -904,7 +907,7 @@
         <v>78</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -915,15 +918,18 @@
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:5" s="4" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="C7" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>122</v>
+      <c r="E7" s="4" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -939,13 +945,13 @@
         <v>85</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>86</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -953,13 +959,13 @@
         <v>87</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>90</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -967,13 +973,13 @@
         <v>88</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>89</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -981,10 +987,10 @@
         <v>91</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -992,13 +998,13 @@
         <v>92</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>93</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1006,7 +1012,7 @@
         <v>94</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>95</v>
@@ -1017,7 +1023,7 @@
         <v>96</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="16" spans="1:5" s="5" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1025,7 +1031,7 @@
         <v>97</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="17" spans="1:5" s="6" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1033,10 +1039,10 @@
         <v>98</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1044,7 +1050,7 @@
         <v>99</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>100</v>
@@ -1055,7 +1061,7 @@
         <v>101</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>64</v>
@@ -1066,7 +1072,7 @@
         <v>102</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>65</v>
@@ -1077,7 +1083,7 @@
         <v>103</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>104</v>
@@ -1088,7 +1094,7 @@
         <v>105</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>114</v>
@@ -1099,7 +1105,7 @@
         <v>106</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1112,7 +1118,7 @@
         <v>108</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>56</v>
@@ -1123,7 +1129,7 @@
         <v>109</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>59</v>

</xml_diff>